<commit_message>
08.12.24,delete search EmployeeID and pager, add search MAIL, update info.xlsx
</commit_message>
<xml_diff>
--- a/Main Modul/info.xlsx
+++ b/Main Modul/info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12330"/>
+    <workbookView windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="343">
   <si>
     <t>Отдел</t>
   </si>
@@ -1040,6 +1040,12 @@
   </si>
   <si>
     <t>Главный специалист по охране труда и пожарной безопасности</t>
+  </si>
+  <si>
+    <t>ООАРП - СУПЕРМАРКЕТЫ</t>
+  </si>
+  <si>
+    <t>МЕНЕДЖЕРЫ ПО ЗАКУПУ (РЦ)</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1058,7 @@
     <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1085,6 +1091,13 @@
       <name val="Calibri"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1556,31 +1569,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1589,119 +1599,122 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1732,6 +1745,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2051,18 +2065,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N511"/>
+  <dimension ref="A1:N516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A284" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A504" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B300" sqref="B300"/>
+      <selection pane="bottomLeft" activeCell="B517" sqref="B517"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="37.8571428571429" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
+    <col min="2" max="2" width="63.8571428571429" customWidth="1"/>
     <col min="3" max="3" width="13.8571428571429" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="13.7142857142857" customWidth="1"/>
@@ -12355,7 +12369,7 @@
       <c r="D284" s="5"/>
       <c r="E284" s="5"/>
     </row>
-    <row r="285" spans="1:5">
+    <row r="285" spans="1:14">
       <c r="A285" s="7"/>
       <c r="B285" s="10" t="s">
         <v>230</v>
@@ -12363,6 +12377,30 @@
       <c r="C285" s="5"/>
       <c r="D285" s="5"/>
       <c r="E285" s="5"/>
+      <c r="G285">
+        <v>0</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+      <c r="I285">
+        <v>0</v>
+      </c>
+      <c r="J285">
+        <v>0</v>
+      </c>
+      <c r="K285">
+        <v>0</v>
+      </c>
+      <c r="L285">
+        <v>0</v>
+      </c>
+      <c r="M285">
+        <v>0</v>
+      </c>
+      <c r="N285">
+        <v>0</v>
+      </c>
     </row>
     <row r="286" spans="1:14">
       <c r="A286" s="6"/>
@@ -13562,6 +13600,9 @@
       </c>
       <c r="E315">
         <v>0</v>
+      </c>
+      <c r="F315" t="s">
+        <v>18</v>
       </c>
       <c r="G315">
         <v>0</v>
@@ -20613,6 +20654,16 @@
       </c>
       <c r="N511">
         <v>1</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1">
+      <c r="A513" s="12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1">
+      <c r="A516" s="12" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>